<commit_message>
Fixed parser, output, generate of url
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Open link to long URL having length of 1554 characters.</t>
+    <t>Open link to long URL having length of 1552 characters.</t>
   </si>
 </sst>
 </file>
@@ -69,7 +69,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>